<commit_message>
added bls and census data
</commit_message>
<xml_diff>
--- a/Data/Data_Source_Tracker.xlsx
+++ b/Data/Data_Source_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laslo\OneDrive\Documents\Maria\Project2_Economic_Disaster\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekhagman/Desktop/Project2_Economic_Disaster/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC10482EE91D75005ADE58ED" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3B120384-4314-4169-8225-501E41E341F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154B700B-177B-A246-8FE8-8DD7C859BCAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="396" windowWidth="22476" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9460" yWindow="1460" windowWidth="22480" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>https://www.kaggle.com/jayrav13/unemployment-by-county-us/downloads/unemployment-by-county-us.zip/2</t>
   </si>
@@ -37,13 +37,85 @@
   </si>
   <si>
     <t>Site</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/lau/laucnty13.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/lau/laucnty14.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/lau/laucnty15.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/lau/laucnty16.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/lau/laucnty17.xlsx</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/lau/laucnty18.xlsx</t>
+  </si>
+  <si>
+    <t>bureau of labor statistics_employment/unemployment by state_2013</t>
+  </si>
+  <si>
+    <t>bureau of labor statistics_employment/unemployment by state_2014</t>
+  </si>
+  <si>
+    <t>bureau of labor statistics_employment/unemployment by state_2015</t>
+  </si>
+  <si>
+    <t>bureau of labor statistics_employment/unemployment by state_2016</t>
+  </si>
+  <si>
+    <t>bureau of labor statistics_employment/unemployment by state_2017</t>
+  </si>
+  <si>
+    <t>bureau of labor statistics_employment/unemployment by state_2018</t>
+  </si>
+  <si>
+    <t>Census Bureau_2013</t>
+  </si>
+  <si>
+    <t>Census Bureau_2014</t>
+  </si>
+  <si>
+    <t>Census Bureau_2015</t>
+  </si>
+  <si>
+    <t>Census Bureau_2016</t>
+  </si>
+  <si>
+    <t>Census Bureau_2017</t>
+  </si>
+  <si>
+    <t>Census Bureau_2018</t>
+  </si>
+  <si>
+    <t>https://www2.census.gov/geo/tiger/GENZ2013/shp/cb_2013_us_county_20m.zip</t>
+  </si>
+  <si>
+    <t>https://www2.census.gov/geo/tiger/GENZ2014/shp/cb_2014_us_county_20m.zip</t>
+  </si>
+  <si>
+    <t>https://www2.census.gov/geo/tiger/GENZ2015/shp/cb_2015_us_county_20m.zip</t>
+  </si>
+  <si>
+    <t>https://www2.census.gov/geo/tiger/GENZ2016/shp/cb_2016_us_county_20m.zip</t>
+  </si>
+  <si>
+    <t>https://www2.census.gov/geo/tiger/GENZ2017/shp/cb_2017_us_county_20m.zip</t>
+  </si>
+  <si>
+    <t>https://www2.census.gov/geo/tiger/GENZ2018/shp/cb_2018_us_county_20m.zip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +130,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,9 +170,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -365,17 +466,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.83203125" customWidth="1"/>
+    <col min="2" max="2" width="93.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -383,17 +486,117 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{AA9A91BB-4010-45E7-AB40-592E3D2B5026}"/>
+    <hyperlink ref="B10" r:id="rId2" display="https://www2.census.gov/geo/tiger/GENZ2013/cb_2013_us_county_20m.zip" xr:uid="{F7C8E9D6-BE66-724B-A387-F196978EF1F7}"/>
+    <hyperlink ref="B11" r:id="rId3" xr:uid="{81C52094-1BFA-5E44-AE3E-54211015ABA4}"/>
+    <hyperlink ref="B12" r:id="rId4" xr:uid="{C66297D9-88C2-2741-9D26-D912F272544C}"/>
+    <hyperlink ref="B13" r:id="rId5" xr:uid="{982A17D5-FCAE-0442-8516-7D2DB8C397E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Small change to source tracker
</commit_message>
<xml_diff>
--- a/Data/Data_Source_Tracker.xlsx
+++ b/Data/Data_Source_Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/derekhagman/Desktop/Project2_Economic_Disaster/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laslo\OneDrive\Documents\Maria\Project2_Economic_Disaster\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154B700B-177B-A246-8FE8-8DD7C859BCAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{280D547C-1460-4C82-B3BB-69D7796DF18D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="1460" windowWidth="22480" windowHeight="11200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="396" windowWidth="22476" windowHeight="11196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,13 +472,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.83203125" customWidth="1"/>
-    <col min="2" max="2" width="93.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.77734375" customWidth="1"/>
+    <col min="2" max="2" width="93.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -486,7 +486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -494,7 +494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -502,7 +502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -510,7 +510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -526,7 +526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -542,7 +542,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -550,7 +550,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -558,7 +558,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -566,7 +566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -574,7 +574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -582,7 +582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>21</v>
       </c>

</xml_diff>